<commit_message>
Unified file clases in the class page
</commit_message>
<xml_diff>
--- a/semilla_Java_POM/src/test/resources/writefiles/test.xlsx
+++ b/semilla_Java_POM/src/test/resources/writefiles/test.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>dresses</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>7 results have been found.</t>
+  </si>
+  <si>
+    <t>0 results have been found.</t>
+  </si>
+  <si>
+    <t>1 result has been found.</t>
+  </si>
+  <si>
+    <t>4 results have been found.</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,16 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New items for search was added and these results
</commit_message>
<xml_diff>
--- a/semilla_Java_POM/src/test/resources/writefiles/test.xlsx
+++ b/semilla_Java_POM/src/test/resources/writefiles/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.romero\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.romero\git\KatalonR_Tests_Java_POM\semilla_Java_POM\src\test\resources\writefiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18AC3A14-77BB-4E24-96C0-A3B8924B31D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921C174C-5D75-4B53-ACE4-BD02390D73A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18680" yWindow="520" windowWidth="14400" windowHeight="7810" xr2:uid="{23F1483B-EF9C-4BCE-A105-078F3AEFE4C9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>dresses</t>
   </si>
@@ -49,13 +49,19 @@
     <t>7 results have been found.</t>
   </si>
   <si>
+    <t>1 result has been found.</t>
+  </si>
+  <si>
+    <t>4 results have been found.</t>
+  </si>
+  <si>
+    <t>jackets</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
     <t>0 results have been found.</t>
-  </si>
-  <si>
-    <t>1 result has been found.</t>
-  </si>
-  <si>
-    <t>4 results have been found.</t>
   </si>
 </sst>
 </file>
@@ -408,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F9637D-BAB7-4DA1-A931-212276D9085B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,20 +430,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>